<commit_message>
More references urls, checking errors in paper added and cuckoo with window code added.
</commit_message>
<xml_diff>
--- a/experiments_data.xlsx
+++ b/experiments_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>L_max/Cuckoo</t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t>NumElems/L_max</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
   </si>
   <si>
     <t>Avg</t>
@@ -170,6 +164,63 @@
   </si>
   <si>
     <t>d/k</t>
+  </si>
+  <si>
+    <t>Moves</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>10^5 repetitions</t>
+  </si>
+  <si>
+    <t>&lt;0.1%</t>
+  </si>
+  <si>
+    <t>&lt;0.2%</t>
+  </si>
+  <si>
+    <t>&lt;0.3%</t>
+  </si>
+  <si>
+    <t>&lt;0.4%</t>
+  </si>
+  <si>
+    <t>&lt;0.5%</t>
+  </si>
+  <si>
+    <t>&lt;0.6%</t>
+  </si>
+  <si>
+    <t>&lt;0.7%</t>
+  </si>
+  <si>
+    <t>&lt;0.9%</t>
+  </si>
+  <si>
+    <t>&gt;=0.9%</t>
+  </si>
+  <si>
+    <t>&lt;0.8%</t>
+  </si>
+  <si>
+    <t>11.56% - 49.77%</t>
+  </si>
+  <si>
+    <t>03.29% - 92.39%</t>
+  </si>
+  <si>
+    <t>00.34% - 97.65%</t>
+  </si>
+  <si>
+    <t>00.20% - 98.00%</t>
+  </si>
+  <si>
+    <t>00.19% - 98.03%</t>
+  </si>
+  <si>
+    <t>00.19% - 98.04%</t>
   </si>
 </sst>
 </file>
@@ -377,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -418,6 +469,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,25 +709,25 @@
             <c:strLit>
               <c:ptCount val="7"/>
               <c:pt idx="0">
-                <c:v>100%</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>200%</c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>300%</c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>400%</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>500%</c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>600%</c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>700%</c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -750,25 +805,25 @@
             <c:strLit>
               <c:ptCount val="7"/>
               <c:pt idx="0">
-                <c:v>100.00%</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>200.00%</c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>300.00%</c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>400.00%</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>500.00%</c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>600.00%</c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>700.00%</c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -846,34 +901,34 @@
             <c:strLit>
               <c:ptCount val="7"/>
               <c:pt idx="0">
-                <c:v>100.00%</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>200.00%</c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>300.00%</c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>400.00%</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>500.00%</c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>600.00%</c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>700.00%</c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>800.00%</c:v>
+                <c:v>8</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>900.00%</c:v>
+                <c:v>9</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>1000.00%</c:v>
+                <c:v>10</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -951,34 +1006,34 @@
             <c:strLit>
               <c:ptCount val="7"/>
               <c:pt idx="0">
-                <c:v>100%</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>200%</c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>300%</c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>400%</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>500%</c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>600%</c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>700%</c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>800%</c:v>
+                <c:v>8</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>900%</c:v>
+                <c:v>9</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>1000%</c:v>
+                <c:v>10</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -1140,11 +1195,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="15287616"/>
-        <c:axId val="15297408"/>
+        <c:axId val="-1471787632"/>
+        <c:axId val="-1471778928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15287616"/>
+        <c:axId val="-1471787632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,7 +1306,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15297408"/>
+        <c:crossAx val="-1471778928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1259,7 +1314,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15297408"/>
+        <c:axId val="-1471778928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1372,7 +1427,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15287616"/>
+        <c:crossAx val="-1471787632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1564,7 +1619,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$51</c:f>
+              <c:f>Sheet1!$K$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1587,7 +1642,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$53:$R$59</c:f>
+              <c:f>Sheet1!$K$53:$K$59</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1622,7 +1677,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$51</c:f>
+              <c:f>Sheet1!$N$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1645,7 +1700,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$53:$U$59</c:f>
+              <c:f>Sheet1!$N$53:$N$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1680,7 +1735,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$V$51</c:f>
+              <c:f>Sheet1!$O$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1703,7 +1758,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$V$53:$V$59</c:f>
+              <c:f>Sheet1!$O$53:$O$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1738,7 +1793,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$W$51</c:f>
+              <c:f>Sheet1!$P$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1761,7 +1816,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$W$53:$W$59</c:f>
+              <c:f>Sheet1!$P$53:$P$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1796,7 +1851,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$51</c:f>
+              <c:f>Sheet1!$M$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1819,7 +1874,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$53:$T$59</c:f>
+              <c:f>Sheet1!$M$53:$M$59</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1854,7 +1909,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$51</c:f>
+              <c:f>Sheet1!$L$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1877,7 +1932,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$53:$S$59</c:f>
+              <c:f>Sheet1!$L$53:$L$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1916,11 +1971,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="15287072"/>
-        <c:axId val="15292512"/>
+        <c:axId val="-1471784368"/>
+        <c:axId val="-1471787088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15287072"/>
+        <c:axId val="-1471784368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2026,7 +2081,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15292512"/>
+        <c:crossAx val="-1471787088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2034,7 +2089,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15292512"/>
+        <c:axId val="-1471787088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2146,7 +2201,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15287072"/>
+        <c:crossAx val="-1471784368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2710,11 +2765,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="15294144"/>
-        <c:axId val="15282176"/>
+        <c:axId val="-1471947248"/>
+        <c:axId val="-1471946160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15294144"/>
+        <c:axId val="-1471947248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2821,7 +2876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15282176"/>
+        <c:crossAx val="-1471946160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2829,7 +2884,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15282176"/>
+        <c:axId val="-1471946160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2949,7 +3004,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15294144"/>
+        <c:crossAx val="-1471947248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3503,11 +3558,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="15139040"/>
-        <c:axId val="235152272"/>
+        <c:axId val="-1280096560"/>
+        <c:axId val="-1280098192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15139040"/>
+        <c:axId val="-1280096560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3613,7 +3668,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="235152272"/>
+        <c:crossAx val="-1280098192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3622,7 +3677,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235152272"/>
+        <c:axId val="-1280098192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3734,7 +3789,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15139040"/>
+        <c:crossAx val="-1280096560"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3787,6 +3842,977 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.9025371828521433E-2"/>
+          <c:y val="3.9428962781649465E-2"/>
+          <c:w val="0.87041907261592311"/>
+          <c:h val="0.54519735576891637"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(2,2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$43:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>&lt;0.1%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&lt;0.2%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>&lt;0.3%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>&lt;0.4%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&lt;0.5%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>&lt;0.6%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>&lt;0.7%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>&lt;0.8%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>&lt;0.9%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>&gt;=0.9%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$43:$C$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(2,4)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$43:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>&lt;0.1%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&lt;0.2%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>&lt;0.3%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>&lt;0.4%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&lt;0.5%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>&lt;0.6%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>&lt;0.7%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>&lt;0.8%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>&lt;0.9%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>&gt;=0.9%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$43:$D$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9465</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(2,8)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$43:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>&lt;0.1%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&lt;0.2%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>&lt;0.3%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>&lt;0.4%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&lt;0.5%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>&lt;0.6%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>&lt;0.7%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>&lt;0.8%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>&lt;0.9%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>&gt;=0.9%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$43:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9861</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(3,2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$43:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>&lt;0.1%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&lt;0.2%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>&lt;0.3%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>&lt;0.4%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&lt;0.5%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>&lt;0.6%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>&lt;0.7%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>&lt;0.8%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>&lt;0.9%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>&gt;=0.9%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$43:$F$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>8002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(3,4)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$43:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>&lt;0.1%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&lt;0.2%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>&lt;0.3%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>&lt;0.4%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&lt;0.5%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>&lt;0.6%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>&lt;0.7%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>&lt;0.8%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>&lt;0.9%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>&gt;=0.9%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$43:$G$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9670</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(3,8)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$43:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>&lt;0.1%</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&lt;0.2%</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>&lt;0.3%</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>&lt;0.4%</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&lt;0.5%</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>&lt;0.6%</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>&lt;0.7%</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>&lt;0.8%</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>&lt;0.9%</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>&gt;=0.9%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$43:$H$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1235967728"/>
+        <c:axId val="-1235967184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1235967728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>distance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to avg</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.80218044619422579"/>
+              <c:y val="0.52562792638749534"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1235967184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1235967184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Counter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1235967728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3984,6 +5010,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -5695,6 +6761,509 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6083,15 +7652,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6165,6 +7734,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6460,47 +8059,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:X160"/>
+  <dimension ref="A2:W160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="J31" workbookViewId="0">
+      <selection activeCell="Z47" sqref="Z47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="20" max="20" width="10.28515625" customWidth="1"/>
+    <col min="22" max="22" width="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -6508,7 +8108,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2">
         <v>0.49719999999999998</v>
@@ -6537,7 +8137,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5">
         <v>0.8296</v>
@@ -6566,39 +8166,39 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="H7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="10">
         <v>1</v>
@@ -7046,37 +8646,37 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="H24" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H24" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="L24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M24" s="7" t="s">
         <v>10</v>
@@ -7108,7 +8708,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B25" s="10">
         <v>1</v>
@@ -7541,7 +9141,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B33" s="10">
         <v>9</v>
       </c>
@@ -7570,7 +9170,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>10</v>
       </c>
@@ -7599,7 +9199,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>11</v>
       </c>
@@ -7628,7 +9228,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="36" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
         <v>12</v>
       </c>
@@ -7657,7 +9257,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B37" s="10">
         <v>13</v>
       </c>
@@ -7686,7 +9286,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B38" s="10">
         <v>14</v>
       </c>
@@ -7715,7 +9315,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="39" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
         <v>15</v>
       </c>
@@ -7744,58 +9344,76 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" t="s">
+        <v>21</v>
+      </c>
+      <c r="K41" t="s">
+        <v>13</v>
+      </c>
+      <c r="L41" t="s">
         <v>14</v>
       </c>
-      <c r="J41" t="s">
+      <c r="M41" t="s">
+        <v>15</v>
+      </c>
+      <c r="N41" t="s">
+        <v>17</v>
+      </c>
+      <c r="O41" t="s">
+        <v>18</v>
+      </c>
+      <c r="P41" t="s">
+        <v>19</v>
+      </c>
+      <c r="R41" t="s">
+        <v>13</v>
+      </c>
+      <c r="S41" t="s">
+        <v>14</v>
+      </c>
+      <c r="T41" t="s">
+        <v>15</v>
+      </c>
+      <c r="U41" t="s">
+        <v>17</v>
+      </c>
+      <c r="V41" t="s">
+        <v>18</v>
+      </c>
+      <c r="W41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C42" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="K41" t="s">
-        <v>15</v>
-      </c>
-      <c r="L41" t="s">
-        <v>16</v>
-      </c>
-      <c r="M41" t="s">
-        <v>17</v>
-      </c>
-      <c r="N41" t="s">
-        <v>19</v>
-      </c>
-      <c r="O41" t="s">
-        <v>20</v>
-      </c>
-      <c r="P41" t="s">
-        <v>21</v>
-      </c>
-      <c r="R41" t="s">
-        <v>15</v>
-      </c>
-      <c r="S41" t="s">
-        <v>16</v>
-      </c>
-      <c r="T41" t="s">
-        <v>17</v>
-      </c>
-      <c r="U41" t="s">
-        <v>19</v>
-      </c>
-      <c r="V41" t="s">
-        <v>20</v>
-      </c>
-      <c r="W41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="G42" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" s="24" t="s">
+        <v>25</v>
+      </c>
       <c r="K42" s="22" t="s">
         <v>11</v>
       </c>
       <c r="L42" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M42" s="23" t="s">
+      <c r="M42" s="24" t="s">
         <v>11</v>
       </c>
       <c r="N42" s="24" t="s">
@@ -7808,701 +9426,755 @@
         <v>11</v>
       </c>
       <c r="R42" s="22" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="S42" s="23" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="T42" s="24" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="U42" s="24" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="V42" s="24" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="W42" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="42">
+        <v>7658</v>
+      </c>
+      <c r="D43" s="20">
+        <v>9465</v>
+      </c>
+      <c r="E43" s="20">
+        <v>9861</v>
+      </c>
+      <c r="F43" s="20">
+        <v>8002</v>
+      </c>
+      <c r="G43" s="20">
+        <v>9670</v>
+      </c>
+      <c r="H43" s="34">
+        <v>10000</v>
+      </c>
       <c r="J43" s="25">
         <v>1</v>
       </c>
       <c r="K43" s="19">
-        <v>0.1138</v>
+        <v>0.23150000000000001</v>
       </c>
       <c r="L43" s="2">
-        <v>0.1208</v>
+        <v>0.23130000000000001</v>
       </c>
       <c r="M43" s="2">
-        <v>0.12889999999999999</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="N43" s="2">
-        <v>9.2299999999999993E-2</v>
-      </c>
-      <c r="O43" s="2">
-        <v>0.36399999999999999</v>
+        <v>0.2301</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="P43" s="4">
-        <v>0.35759999999999997</v>
-      </c>
-      <c r="R43" s="19">
-        <v>0.23150000000000001</v>
-      </c>
-      <c r="S43" s="2">
-        <v>0.23130000000000001</v>
-      </c>
-      <c r="T43" s="2">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="U43" s="2">
-        <v>0.2301</v>
-      </c>
-      <c r="V43" s="2">
-        <v>0.49590000000000001</v>
-      </c>
-      <c r="W43" s="4">
         <v>0.49880000000000002</v>
       </c>
-      <c r="X43" s="1"/>
-    </row>
-    <row r="44" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Q43" s="1"/>
+      <c r="R43" s="26">
+        <v>0</v>
+      </c>
+      <c r="S43" s="32">
+        <v>0</v>
+      </c>
+      <c r="T43" s="32">
+        <v>0</v>
+      </c>
+      <c r="U43" s="32">
+        <v>0</v>
+      </c>
+      <c r="V43" s="32">
+        <v>0</v>
+      </c>
+      <c r="W43" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="42">
+        <v>1571</v>
+      </c>
+      <c r="D44" s="20">
+        <v>529</v>
+      </c>
+      <c r="E44" s="20">
+        <v>135</v>
+      </c>
+      <c r="F44" s="20">
+        <v>1105</v>
+      </c>
+      <c r="G44" s="20">
+        <v>279</v>
+      </c>
+      <c r="H44" s="34">
+        <v>0</v>
+      </c>
       <c r="J44" s="25">
         <v>2</v>
       </c>
       <c r="K44" s="19">
-        <v>0.81410000000000005</v>
+        <v>0.95820000000000005</v>
       </c>
       <c r="L44" s="2">
-        <v>0.53239999999999998</v>
+        <v>0.71589999999999998</v>
       </c>
       <c r="M44" s="2">
-        <v>0.65159999999999996</v>
+        <v>0.80489999999999995</v>
       </c>
       <c r="N44" s="2">
-        <v>0.92010000000000003</v>
-      </c>
-      <c r="O44" s="2">
-        <v>0.89190000000000003</v>
+        <v>0.95540000000000003</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="P44" s="4">
-        <v>0.88370000000000004</v>
-      </c>
-      <c r="R44" s="19">
-        <v>0.95820000000000005</v>
-      </c>
-      <c r="S44" s="2">
-        <v>0.71589999999999998</v>
-      </c>
-      <c r="T44" s="2">
-        <v>0.80489999999999995</v>
-      </c>
-      <c r="U44" s="2">
-        <v>0.95540000000000003</v>
-      </c>
-      <c r="V44" s="2">
-        <v>0.92420000000000002</v>
-      </c>
-      <c r="W44" s="4">
         <v>0.91810000000000003</v>
       </c>
-      <c r="X44" s="1"/>
-    </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Q44" s="1"/>
+      <c r="R44" s="26">
+        <v>0.19</v>
+      </c>
+      <c r="S44" s="32">
+        <v>0.03</v>
+      </c>
+      <c r="T44" s="32">
+        <v>0.06</v>
+      </c>
+      <c r="U44" s="32">
+        <v>0.21</v>
+      </c>
+      <c r="V44" s="32">
+        <v>0.15</v>
+      </c>
+      <c r="W44" s="40">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B45" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="42">
+        <v>602</v>
+      </c>
+      <c r="D45" s="20">
+        <v>6</v>
+      </c>
+      <c r="E45" s="20">
+        <v>4</v>
+      </c>
+      <c r="F45" s="20">
+        <v>501</v>
+      </c>
+      <c r="G45" s="20">
+        <v>36</v>
+      </c>
+      <c r="H45" s="34">
+        <v>0</v>
+      </c>
       <c r="J45" s="25">
         <v>3</v>
       </c>
       <c r="K45" s="19">
-        <v>0.97809999999999997</v>
+        <v>0.98019999999999996</v>
       </c>
       <c r="L45" s="2">
-        <v>0.88829999999999998</v>
+        <v>0.93440000000000001</v>
       </c>
       <c r="M45" s="2">
-        <v>0.93410000000000004</v>
+        <v>0.96240000000000003</v>
       </c>
       <c r="N45" s="2">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="O45" s="2">
-        <v>0.97270000000000001</v>
+        <v>0.98</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="P45" s="4">
-        <v>0.97099999999999997</v>
-      </c>
-      <c r="R45" s="19">
-        <v>0.98019999999999996</v>
-      </c>
-      <c r="S45" s="2">
-        <v>0.93440000000000001</v>
-      </c>
-      <c r="T45" s="2">
-        <v>0.96240000000000003</v>
-      </c>
-      <c r="U45" s="2">
-        <v>0.98</v>
-      </c>
-      <c r="V45" s="2">
-        <v>0.97640000000000005</v>
-      </c>
-      <c r="W45" s="4">
         <v>0.97519999999999996</v>
       </c>
-      <c r="X45" s="1"/>
-    </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Q45" s="1"/>
+      <c r="R45" s="26">
+        <v>0.93</v>
+      </c>
+      <c r="S45" s="32">
+        <v>0.35</v>
+      </c>
+      <c r="T45" s="32">
+        <v>0.54</v>
+      </c>
+      <c r="U45" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="V45" s="32">
+        <v>0.72</v>
+      </c>
+      <c r="W45" s="40">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B46" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="42">
+        <v>149</v>
+      </c>
+      <c r="D46" s="20">
+        <v>0</v>
+      </c>
+      <c r="E46" s="20">
+        <v>0</v>
+      </c>
+      <c r="F46" s="20">
+        <v>200</v>
+      </c>
+      <c r="G46" s="20">
+        <v>9</v>
+      </c>
+      <c r="H46" s="34">
+        <v>0</v>
+      </c>
       <c r="J46" s="25">
         <v>4</v>
       </c>
       <c r="K46" s="19">
-        <v>0.97829999999999995</v>
+        <v>0.98040000000000005</v>
       </c>
       <c r="L46" s="2">
-        <v>0.96860000000000002</v>
+        <v>0.97489999999999999</v>
       </c>
       <c r="M46" s="2">
-        <v>0.97599999999999998</v>
+        <v>0.97870000000000001</v>
       </c>
       <c r="N46" s="2">
-        <v>0.97829999999999995</v>
-      </c>
-      <c r="O46" s="2">
-        <v>0.9778</v>
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="P46" s="4">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="R46" s="19">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="S46" s="2">
-        <v>0.97489999999999999</v>
-      </c>
-      <c r="T46" s="2">
-        <v>0.97870000000000001</v>
-      </c>
-      <c r="U46" s="2">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="V46" s="2">
+        <v>0.97989999999999999</v>
+      </c>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="26">
+        <v>1.62</v>
+      </c>
+      <c r="S46" s="32">
         <v>0.98</v>
       </c>
-      <c r="W46" s="4">
-        <v>0.97989999999999999</v>
-      </c>
-      <c r="X46" s="1"/>
-    </row>
-    <row r="47" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T46" s="32">
+        <v>1.19</v>
+      </c>
+      <c r="U46" s="32">
+        <v>1.57</v>
+      </c>
+      <c r="V46" s="32">
+        <v>1.37</v>
+      </c>
+      <c r="W46" s="40">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B47" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="42">
+        <v>19</v>
+      </c>
+      <c r="D47" s="20">
+        <v>0</v>
+      </c>
+      <c r="E47" s="20">
+        <v>0</v>
+      </c>
+      <c r="F47" s="20">
+        <v>104</v>
+      </c>
+      <c r="G47" s="20">
+        <v>3</v>
+      </c>
+      <c r="H47" s="34">
+        <v>0</v>
+      </c>
       <c r="J47" s="25">
         <v>5</v>
       </c>
       <c r="K47" s="19">
-        <v>0.97829999999999995</v>
+        <v>0.98040000000000005</v>
       </c>
       <c r="L47" s="2">
-        <v>0.97750000000000004</v>
+        <v>0.97970000000000002</v>
       </c>
       <c r="M47" s="2">
-        <v>0.97829999999999995</v>
+        <v>0.98019999999999996</v>
       </c>
       <c r="N47" s="2">
-        <v>0.97829999999999995</v>
-      </c>
-      <c r="O47" s="2">
-        <v>0.97809999999999997</v>
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="P47" s="4">
-        <v>0.97850000000000004</v>
-      </c>
-      <c r="R47" s="19">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="S47" s="2">
-        <v>0.97970000000000002</v>
-      </c>
-      <c r="T47" s="2">
-        <v>0.98019999999999996</v>
-      </c>
-      <c r="U47" s="2">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="V47" s="2">
         <v>0.98029999999999995</v>
       </c>
-      <c r="W47" s="4">
-        <v>0.98029999999999995</v>
-      </c>
-      <c r="X47" s="1"/>
-    </row>
-    <row r="48" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Q47" s="1"/>
+      <c r="R47" s="26">
+        <v>2.35</v>
+      </c>
+      <c r="S47" s="32">
+        <v>1.73</v>
+      </c>
+      <c r="T47" s="32">
+        <v>1.89</v>
+      </c>
+      <c r="U47" s="32">
+        <v>2.27</v>
+      </c>
+      <c r="V47" s="32">
+        <v>2.06</v>
+      </c>
+      <c r="W47" s="40">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B48" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="42">
+        <v>1</v>
+      </c>
+      <c r="D48" s="20">
+        <v>0</v>
+      </c>
+      <c r="E48" s="20">
+        <v>0</v>
+      </c>
+      <c r="F48" s="20">
+        <v>40</v>
+      </c>
+      <c r="G48" s="20">
+        <v>1</v>
+      </c>
+      <c r="H48" s="34">
+        <v>0</v>
+      </c>
       <c r="J48" s="25">
         <v>6</v>
       </c>
       <c r="K48" s="19">
-        <v>0.97829999999999995</v>
+        <v>0.98040000000000005</v>
       </c>
       <c r="L48" s="2">
-        <v>0.97840000000000005</v>
+        <v>0.98029999999999995</v>
       </c>
       <c r="M48" s="2">
-        <v>0.97860000000000003</v>
+        <v>0.98040000000000005</v>
       </c>
       <c r="N48" s="2">
-        <v>0.97829999999999995</v>
-      </c>
-      <c r="O48" s="2">
-        <v>0.97819999999999996</v>
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="P48" s="4">
-        <v>0.97860000000000003</v>
-      </c>
-      <c r="R48" s="19">
         <v>0.98040000000000005</v>
       </c>
-      <c r="S48" s="2">
-        <v>0.98029999999999995</v>
-      </c>
-      <c r="T48" s="2">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="U48" s="2">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="V48" s="2">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="W48" s="4">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="X48" s="1"/>
-    </row>
-    <row r="49" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="Q48" s="1"/>
+      <c r="R48" s="26">
+        <v>3.05</v>
+      </c>
+      <c r="S48" s="32">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="T48" s="32">
+        <v>2.58</v>
+      </c>
+      <c r="U48" s="32">
+        <v>2.95</v>
+      </c>
+      <c r="V48" s="32">
+        <v>2.74</v>
+      </c>
+      <c r="W48" s="40">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B49" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="42">
+        <v>0</v>
+      </c>
+      <c r="D49" s="20">
+        <v>0</v>
+      </c>
+      <c r="E49" s="20">
+        <v>0</v>
+      </c>
+      <c r="F49" s="20">
+        <v>20</v>
+      </c>
+      <c r="G49" s="20">
+        <v>0</v>
+      </c>
+      <c r="H49" s="34">
+        <v>0</v>
+      </c>
       <c r="J49" s="25">
         <v>7</v>
       </c>
       <c r="K49" s="17">
-        <v>0.97829999999999995</v>
+        <v>0.98040000000000005</v>
       </c>
       <c r="L49" s="5">
-        <v>0.97840000000000005</v>
+        <v>0.98040000000000005</v>
       </c>
       <c r="M49" s="5">
-        <v>0.97860000000000003</v>
+        <v>0.98040000000000005</v>
       </c>
       <c r="N49" s="5">
-        <v>0.97829999999999995</v>
-      </c>
-      <c r="O49" s="5">
-        <v>0.97819999999999996</v>
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="O49" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="P49" s="6">
-        <v>0.97860000000000003</v>
-      </c>
-      <c r="R49" s="17">
         <v>0.98040000000000005</v>
       </c>
-      <c r="S49" s="5">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="T49" s="5">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="U49" s="5">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="V49" s="5">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="W49" s="6">
-        <v>0.98040000000000005</v>
-      </c>
-      <c r="X49" s="1"/>
-    </row>
-    <row r="50" spans="6:24" x14ac:dyDescent="0.25">
+      <c r="Q49" s="1"/>
+      <c r="R49" s="27">
+        <v>3.76</v>
+      </c>
+      <c r="S49" s="33">
+        <v>3.21</v>
+      </c>
+      <c r="T49" s="33">
+        <v>3.28</v>
+      </c>
+      <c r="U49" s="33">
+        <v>3.64</v>
+      </c>
+      <c r="V49" s="33">
+        <v>3.42</v>
+      </c>
+      <c r="W49" s="41">
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B50" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="42">
+        <v>0</v>
+      </c>
+      <c r="D50" s="20">
+        <v>0</v>
+      </c>
+      <c r="E50" s="20">
+        <v>0</v>
+      </c>
+      <c r="F50" s="20">
+        <v>12</v>
+      </c>
+      <c r="G50" s="20">
+        <v>0</v>
+      </c>
+      <c r="H50" s="34">
+        <v>0</v>
+      </c>
       <c r="M50" s="1"/>
       <c r="P50" s="1"/>
       <c r="T50" s="1"/>
     </row>
-    <row r="51" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B51" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="42">
+        <v>0</v>
+      </c>
+      <c r="D51" s="20">
+        <v>0</v>
+      </c>
+      <c r="E51" s="20">
+        <v>0</v>
+      </c>
+      <c r="F51" s="20">
+        <v>5</v>
+      </c>
+      <c r="G51" s="20">
+        <v>1</v>
+      </c>
+      <c r="H51" s="34">
+        <v>0</v>
+      </c>
       <c r="K51" t="s">
+        <v>13</v>
+      </c>
+      <c r="L51" t="s">
+        <v>14</v>
+      </c>
+      <c r="M51" t="s">
         <v>15</v>
       </c>
-      <c r="L51" t="s">
+      <c r="N51" t="s">
+        <v>17</v>
+      </c>
+      <c r="O51" t="s">
+        <v>18</v>
+      </c>
+      <c r="P51" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B52" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="43">
+        <v>0</v>
+      </c>
+      <c r="D52" s="21">
+        <v>0</v>
+      </c>
+      <c r="E52" s="21">
+        <v>0</v>
+      </c>
+      <c r="F52" s="21">
+        <v>11</v>
+      </c>
+      <c r="G52" s="21">
+        <v>1</v>
+      </c>
+      <c r="H52" s="35">
+        <v>0</v>
+      </c>
+      <c r="K52" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="M51" t="s">
-        <v>17</v>
-      </c>
-      <c r="N51" t="s">
-        <v>19</v>
-      </c>
-      <c r="O51" t="s">
-        <v>20</v>
-      </c>
-      <c r="P51" t="s">
-        <v>21</v>
-      </c>
-      <c r="R51" t="s">
-        <v>15</v>
-      </c>
-      <c r="S51" t="s">
+      <c r="L52" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="T51" t="s">
-        <v>17</v>
-      </c>
-      <c r="U51" t="s">
-        <v>19</v>
-      </c>
-      <c r="V51" t="s">
-        <v>20</v>
-      </c>
-      <c r="W51" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="K52" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="L52" s="23" t="s">
-        <v>12</v>
-      </c>
       <c r="M52" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="N52" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="O52" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="P52" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="R52" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="S52" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="T52" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="U52" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="V52" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="W52" s="36" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="6:24" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="N52" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="O52" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P52" s="36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J53" s="25">
         <v>1</v>
       </c>
-      <c r="K53" s="19">
-        <v>0.31480000000000002</v>
-      </c>
-      <c r="L53" s="2">
-        <v>0.32550000000000001</v>
-      </c>
-      <c r="M53" s="2">
-        <v>0.39360000000000001</v>
-      </c>
-      <c r="N53" s="2">
-        <v>0.32190000000000002</v>
-      </c>
-      <c r="O53" s="2">
-        <v>0.56359999999999999</v>
-      </c>
-      <c r="P53" s="4">
-        <v>0.58020000000000005</v>
-      </c>
-      <c r="R53" s="26">
+      <c r="K53" s="26">
         <v>0.23</v>
       </c>
-      <c r="S53" s="20">
+      <c r="L53" s="20">
         <v>0.23</v>
       </c>
-      <c r="T53" s="32">
+      <c r="M53" s="32">
         <v>0.28999999999999998</v>
       </c>
-      <c r="U53" s="20">
+      <c r="N53" s="20">
         <v>0.23</v>
       </c>
-      <c r="V53" s="20">
+      <c r="O53" s="20">
         <v>0.5</v>
       </c>
-      <c r="W53" s="34">
+      <c r="P53" s="34">
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J54" s="25">
         <v>2</v>
       </c>
-      <c r="K54" s="19">
-        <v>0.97050000000000003</v>
-      </c>
-      <c r="L54" s="2">
-        <v>0.78039999999999998</v>
-      </c>
-      <c r="M54" s="2">
-        <v>0.85940000000000005</v>
-      </c>
-      <c r="N54" s="2">
-        <v>0.96479999999999999</v>
-      </c>
-      <c r="O54" s="2">
-        <v>0.94130000000000003</v>
-      </c>
-      <c r="P54" s="4">
-        <v>0.9335</v>
-      </c>
-      <c r="R54" s="26">
+      <c r="K54" s="26">
         <v>1.28</v>
       </c>
-      <c r="S54" s="20">
+      <c r="L54" s="20">
         <v>0.79</v>
       </c>
-      <c r="T54" s="32">
+      <c r="M54" s="32">
         <v>0.93</v>
       </c>
-      <c r="U54" s="20">
+      <c r="N54" s="20">
         <v>1.3</v>
       </c>
-      <c r="V54" s="20">
+      <c r="O54" s="20">
         <v>1.2</v>
       </c>
-      <c r="W54" s="34">
+      <c r="P54" s="34">
         <v>1.19</v>
       </c>
     </row>
-    <row r="55" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J55" s="25">
         <v>3</v>
       </c>
-      <c r="K55" s="19">
-        <v>0.98229999999999995</v>
-      </c>
-      <c r="L55" s="2">
-        <v>0.9516</v>
-      </c>
-      <c r="M55" s="2">
-        <v>0.96960000000000002</v>
-      </c>
-      <c r="N55" s="2">
-        <v>0.9819</v>
-      </c>
-      <c r="O55" s="2">
-        <v>0.97870000000000001</v>
-      </c>
-      <c r="P55" s="4">
-        <v>0.97809999999999997</v>
-      </c>
-      <c r="R55" s="26">
+      <c r="K55" s="26">
         <v>2.19</v>
       </c>
-      <c r="S55" s="20">
+      <c r="L55" s="20">
         <v>1.43</v>
       </c>
-      <c r="T55" s="32">
+      <c r="M55" s="32">
         <v>1.69</v>
       </c>
-      <c r="U55" s="20">
+      <c r="N55" s="20">
         <v>2.1800000000000002</v>
       </c>
-      <c r="V55" s="20">
+      <c r="O55" s="20">
         <v>1.97</v>
       </c>
-      <c r="W55" s="34">
+      <c r="P55" s="34">
         <v>1.96</v>
       </c>
     </row>
-    <row r="56" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J56" s="25">
         <v>4</v>
       </c>
-      <c r="K56" s="19">
-        <v>0.98240000000000005</v>
-      </c>
-      <c r="L56" s="2">
-        <v>0.97840000000000005</v>
-      </c>
-      <c r="M56" s="2">
-        <v>0.98109999999999997</v>
-      </c>
-      <c r="N56" s="2">
-        <v>0.98219999999999996</v>
-      </c>
-      <c r="O56" s="2">
-        <v>0.98180000000000001</v>
-      </c>
-      <c r="P56" s="4">
-        <v>0.98209999999999997</v>
-      </c>
-      <c r="R56" s="26">
+      <c r="K56" s="26">
         <v>3.03</v>
       </c>
-      <c r="S56" s="20">
+      <c r="L56" s="20">
         <v>2.23</v>
       </c>
-      <c r="T56" s="32">
+      <c r="M56" s="32">
         <v>2.5</v>
       </c>
-      <c r="U56" s="20">
+      <c r="N56" s="20">
         <v>3.01</v>
       </c>
-      <c r="V56" s="20">
+      <c r="O56" s="20">
         <v>2.79</v>
       </c>
-      <c r="W56" s="34">
+      <c r="P56" s="34">
         <v>2.79</v>
       </c>
     </row>
-    <row r="57" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J57" s="25">
         <v>5</v>
       </c>
-      <c r="K57" s="19">
-        <v>0.98240000000000005</v>
-      </c>
-      <c r="L57" s="2">
-        <v>0.98160000000000003</v>
-      </c>
-      <c r="M57" s="2">
-        <v>0.98240000000000005</v>
-      </c>
-      <c r="N57" s="2">
-        <v>0.98219999999999996</v>
-      </c>
-      <c r="O57" s="2">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="P57" s="4">
-        <v>0.98250000000000004</v>
-      </c>
-      <c r="R57" s="26">
+      <c r="K57" s="26">
         <v>3.89</v>
       </c>
-      <c r="S57" s="20">
+      <c r="L57" s="20">
         <v>3.11</v>
       </c>
-      <c r="T57" s="32">
+      <c r="M57" s="32">
         <v>3.35</v>
       </c>
-      <c r="U57" s="20">
+      <c r="N57" s="20">
         <v>3.88</v>
       </c>
-      <c r="V57" s="20">
+      <c r="O57" s="20">
         <v>3.64</v>
       </c>
-      <c r="W57" s="34">
+      <c r="P57" s="34">
         <v>3.65</v>
       </c>
     </row>
-    <row r="58" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J58" s="25">
         <v>6</v>
       </c>
-      <c r="K58" s="19">
-        <v>0.98240000000000005</v>
-      </c>
-      <c r="L58" s="2">
-        <v>0.98219999999999996</v>
-      </c>
-      <c r="M58" s="2">
-        <v>0.98250000000000004</v>
-      </c>
-      <c r="N58" s="2">
-        <v>0.98219999999999996</v>
-      </c>
-      <c r="O58" s="2">
-        <v>0.98209999999999997</v>
-      </c>
-      <c r="P58" s="4">
-        <v>0.98250000000000004</v>
-      </c>
-      <c r="R58" s="26">
+      <c r="K58" s="26">
         <v>4.74</v>
       </c>
-      <c r="S58" s="20">
+      <c r="L58" s="20">
         <v>4.01</v>
       </c>
-      <c r="T58" s="32">
+      <c r="M58" s="32">
         <v>4.21</v>
       </c>
-      <c r="U58" s="20">
+      <c r="N58" s="20">
         <v>4.7300000000000004</v>
       </c>
-      <c r="V58" s="20">
+      <c r="O58" s="20">
         <v>4.5</v>
       </c>
-      <c r="W58" s="34">
+      <c r="P58" s="34">
         <v>4.5</v>
       </c>
     </row>
-    <row r="59" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
       <c r="J59" s="25">
         <v>7</v>
       </c>
-      <c r="K59" s="17">
-        <v>0.98240000000000005</v>
-      </c>
-      <c r="L59" s="5">
-        <v>0.98229999999999995</v>
-      </c>
-      <c r="M59" s="5">
-        <v>0.98260000000000003</v>
-      </c>
-      <c r="N59" s="5">
-        <v>0.98219999999999996</v>
-      </c>
-      <c r="O59" s="5">
-        <v>0.98209999999999997</v>
-      </c>
-      <c r="P59" s="6">
-        <v>0.98250000000000004</v>
-      </c>
-      <c r="R59" s="27">
+      <c r="K59" s="27">
         <v>5.6</v>
       </c>
-      <c r="S59" s="21">
+      <c r="L59" s="21">
         <v>4.8600000000000003</v>
       </c>
-      <c r="T59" s="33">
+      <c r="M59" s="33">
         <v>5.0599999999999996</v>
       </c>
-      <c r="U59" s="21">
+      <c r="N59" s="21">
         <v>5.59</v>
       </c>
-      <c r="V59" s="21">
+      <c r="O59" s="21">
         <v>5.35</v>
       </c>
-      <c r="W59" s="35">
+      <c r="P59" s="35">
         <v>5.36</v>
       </c>
     </row>
-    <row r="62" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
       <c r="F62" t="s">
         <v>4</v>
       </c>
       <c r="G62" s="37"/>
       <c r="H62" s="23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="6:24" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
       <c r="F63" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G63" s="39">
         <v>0</v>
@@ -8514,7 +10186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
       <c r="G64" s="39">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
version 0.2 of paper is up
</commit_message>
<xml_diff>
--- a/experiments_data.xlsx
+++ b/experiments_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>L_max/Cuckoo</t>
   </si>
@@ -222,6 +222,15 @@
   <si>
     <t>00.19% - 98.04%</t>
   </si>
+  <si>
+    <t>moves</t>
+  </si>
+  <si>
+    <t>Table use</t>
+  </si>
+  <si>
+    <t>LL_Global</t>
+  </si>
 </sst>
 </file>
 
@@ -240,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +265,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -473,6 +488,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,25 +629,25 @@
             <c:strLit>
               <c:ptCount val="7"/>
               <c:pt idx="0">
-                <c:v>100.00%</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>200.00%</c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>300.00%</c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>400.00%</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>500.00%</c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>600.00%</c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>700.00%</c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -1111,34 +1127,34 @@
             <c:strLit>
               <c:ptCount val="7"/>
               <c:pt idx="0">
-                <c:v>100.000%</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>200.000%</c:v>
+                <c:v>2</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>300.000%</c:v>
+                <c:v>3</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>400.000%</c:v>
+                <c:v>4</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>500.000%</c:v>
+                <c:v>5</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>600.000%</c:v>
+                <c:v>6</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>700.000%</c:v>
+                <c:v>7</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>800.000%</c:v>
+                <c:v>8</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>900.000%</c:v>
+                <c:v>9</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>1000.000%</c:v>
+                <c:v>10</c:v>
               </c:pt>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
@@ -1195,11 +1211,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1471787632"/>
-        <c:axId val="-1471778928"/>
+        <c:axId val="-1511730224"/>
+        <c:axId val="-1511729680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1471787632"/>
+        <c:axId val="-1511730224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1306,7 +1322,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1471778928"/>
+        <c:crossAx val="-1511729680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1314,7 +1330,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1471778928"/>
+        <c:axId val="-1511729680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1366,7 +1382,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1427,7 +1442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1471787632"/>
+        <c:crossAx val="-1511730224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1531,74 +1546,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Work</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> done</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.4184444444444444"/>
-          <c:y val="0"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1971,11 +1919,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1471784368"/>
-        <c:axId val="-1471787088"/>
+        <c:axId val="-1511717712"/>
+        <c:axId val="-1511726416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1471784368"/>
+        <c:axId val="-1511717712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,7 +2029,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1471787088"/>
+        <c:crossAx val="-1511726416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2089,7 +2037,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1471787088"/>
+        <c:axId val="-1511726416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2201,7 +2149,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1471784368"/>
+        <c:crossAx val="-1511717712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2765,11 +2713,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1471947248"/>
-        <c:axId val="-1471946160"/>
+        <c:axId val="-1511723152"/>
+        <c:axId val="-1511717168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1471947248"/>
+        <c:axId val="-1511723152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2876,7 +2824,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1471946160"/>
+        <c:crossAx val="-1511717168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2884,7 +2832,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1471946160"/>
+        <c:axId val="-1511717168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3004,7 +2952,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1471947248"/>
+        <c:crossAx val="-1511723152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3558,11 +3506,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1280096560"/>
-        <c:axId val="-1280098192"/>
+        <c:axId val="-1511728592"/>
+        <c:axId val="-1511900960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1280096560"/>
+        <c:axId val="-1511728592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3668,7 +3616,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1280098192"/>
+        <c:crossAx val="-1511900960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3677,7 +3625,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1280098192"/>
+        <c:axId val="-1511900960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3789,7 +3737,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1280096560"/>
+        <c:crossAx val="-1511728592"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4532,11 +4480,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1235967728"/>
-        <c:axId val="-1235967184"/>
+        <c:axId val="-1332944416"/>
+        <c:axId val="-1332947680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1235967728"/>
+        <c:axId val="-1332944416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4646,7 +4594,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1235967184"/>
+        <c:crossAx val="-1332947680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4654,7 +4602,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1235967184"/>
+        <c:axId val="-1332947680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -4762,7 +4710,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1235967728"/>
+        <c:crossAx val="-1332944416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4813,6 +4761,1364 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.5914260717410313E-2"/>
+          <c:y val="4.2083333333333355E-2"/>
+          <c:w val="0.87353018372703417"/>
+          <c:h val="0.8736654272382619"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LL_Global</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Y$43:$Y$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$43:$Z$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>91.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>97.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.87</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97.98</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>98.02</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>98.04</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>98.04</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>98.04</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>98.04</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>98.04</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>98.04</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>98.04</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>98.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AC$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LL_LL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Y$43:$Y$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AC$43:$AC$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>90.16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.43</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.82</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97.9</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>97.96</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>98.01</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>98.02</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AD$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LL_Left</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Y$43:$Y$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AD$43:$AD$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>90.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97.61</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>97.75</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>97.84</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>97.9</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>97.94</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>97.97</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>97.99</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>98.01</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>98.02</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>98.02</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AE$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LL_Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Y$43:$Y$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AE$43:$AE$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>89.61</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97.5</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>97.67</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>97.79</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>97.86</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>97.92</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>97.95</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>97.98</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>97.99</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>98.01</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>98.02</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>98.02</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>97.93</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>97.93</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>97.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AB$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random_Global</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Y$43:$Y$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AB$43:$AB$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>85.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>93.56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.76</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97.18</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>97.45</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>97.63</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>97.75</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>97.84</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>97.9</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>97.94</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>97.96</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>97.99</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>98.01</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>98.02</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>98.02</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>98.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AA$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Left Global</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Y$43:$Y$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$43:$AA$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>83.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>89.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92.49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94.29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>96.19</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96.71</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>97.08</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>97.34</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>97.52</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>97.65</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>97.75</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>97.82</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>97.87</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>97.91</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>97.94</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>97.97</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>97.98</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>98.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1332940064"/>
+        <c:axId val="-1332950400"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1332940064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>Moves/item</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.83801946631671054"/>
+              <c:y val="0.8416433362496355"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1332950400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1332950400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="98"/>
+          <c:min val="82"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Table</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> use (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1332940064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.49445056867891524"/>
+          <c:y val="0.38773038786818315"/>
+          <c:w val="0.46943219597550306"/>
+          <c:h val="0.30208442694663173"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5050,6 +6356,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -7264,6 +8610,522 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7764,6 +9626,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8059,10 +9951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:W160"/>
+  <dimension ref="A2:AE160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J31" workbookViewId="0">
-      <selection activeCell="Z47" sqref="Z47"/>
+    <sheetView tabSelected="1" topLeftCell="M52" workbookViewId="0">
+      <selection activeCell="AG45" sqref="AG45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9141,7 +11033,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B33" s="10">
         <v>9</v>
       </c>
@@ -9170,7 +11062,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B34" s="10">
         <v>10</v>
       </c>
@@ -9199,7 +11091,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B35" s="10">
         <v>11</v>
       </c>
@@ -9228,7 +11120,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B36" s="10">
         <v>12</v>
       </c>
@@ -9257,7 +11149,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B37" s="10">
         <v>13</v>
       </c>
@@ -9286,7 +11178,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B38" s="10">
         <v>14</v>
       </c>
@@ -9315,7 +11207,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
         <v>15</v>
       </c>
@@ -9344,7 +11236,7 @@
         <v>0.99999199999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
         <v>12</v>
       </c>
@@ -9387,8 +11279,29 @@
       <c r="W41" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y41" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="C42" s="22" t="s">
         <v>20</v>
       </c>
@@ -9443,8 +11356,29 @@
       <c r="W42" s="24" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y42" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z42" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA42" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB42" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC42" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD42" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE42" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -9509,8 +11443,29 @@
       <c r="W43" s="40">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y43" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="Z43" s="26">
+        <v>91.75</v>
+      </c>
+      <c r="AA43" s="32">
+        <v>83.3</v>
+      </c>
+      <c r="AB43" s="32">
+        <v>85.67</v>
+      </c>
+      <c r="AC43" s="32">
+        <v>90.16</v>
+      </c>
+      <c r="AD43" s="32">
+        <v>90.18</v>
+      </c>
+      <c r="AE43" s="40">
+        <v>89.61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -9575,8 +11530,29 @@
       <c r="W44" s="40">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y44" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="Z44" s="26">
+        <v>96.15</v>
+      </c>
+      <c r="AA44" s="32">
+        <v>89.44</v>
+      </c>
+      <c r="AB44" s="32">
+        <v>90.91</v>
+      </c>
+      <c r="AC44" s="32">
+        <v>95.29</v>
+      </c>
+      <c r="AD44" s="32">
+        <v>93.81</v>
+      </c>
+      <c r="AE44" s="40">
+        <v>93.24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B45" s="25" t="s">
         <v>55</v>
       </c>
@@ -9638,8 +11614,29 @@
       <c r="W45" s="40">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y45" s="25">
+        <v>0.3</v>
+      </c>
+      <c r="Z45" s="26">
+        <v>97.32</v>
+      </c>
+      <c r="AA45" s="32">
+        <v>92.49</v>
+      </c>
+      <c r="AB45" s="32">
+        <v>93.56</v>
+      </c>
+      <c r="AC45" s="32">
+        <v>96.85</v>
+      </c>
+      <c r="AD45" s="32">
+        <v>95.54</v>
+      </c>
+      <c r="AE45" s="40">
+        <v>95.08</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B46" s="25" t="s">
         <v>56</v>
       </c>
@@ -9701,8 +11698,29 @@
       <c r="W46" s="40">
         <v>1.37</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y46" s="25">
+        <v>0.4</v>
+      </c>
+      <c r="Z46" s="26">
+        <v>97.72</v>
+      </c>
+      <c r="AA46" s="32">
+        <v>94.29</v>
+      </c>
+      <c r="AB46" s="32">
+        <v>95.14</v>
+      </c>
+      <c r="AC46" s="32">
+        <v>97.43</v>
+      </c>
+      <c r="AD46" s="32">
+        <v>96.5</v>
+      </c>
+      <c r="AE46" s="40">
+        <v>96.16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B47" s="25" t="s">
         <v>57</v>
       </c>
@@ -9764,8 +11782,29 @@
       <c r="W47" s="40">
         <v>2.06</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y47" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="Z47" s="26">
+        <v>97.87</v>
+      </c>
+      <c r="AA47" s="32">
+        <v>95.43</v>
+      </c>
+      <c r="AB47" s="32">
+        <v>96.13</v>
+      </c>
+      <c r="AC47" s="32">
+        <v>97.68</v>
+      </c>
+      <c r="AD47" s="32">
+        <v>97.06</v>
+      </c>
+      <c r="AE47" s="40">
+        <v>96.83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B48" s="25" t="s">
         <v>58</v>
       </c>
@@ -9827,8 +11866,29 @@
       <c r="W48" s="40">
         <v>2.73</v>
       </c>
-    </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y48" s="25">
+        <v>0.6</v>
+      </c>
+      <c r="Z48" s="26">
+        <v>97.94</v>
+      </c>
+      <c r="AA48" s="32">
+        <v>96.19</v>
+      </c>
+      <c r="AB48" s="32">
+        <v>96.76</v>
+      </c>
+      <c r="AC48" s="32">
+        <v>97.82</v>
+      </c>
+      <c r="AD48" s="32">
+        <v>97.4</v>
+      </c>
+      <c r="AE48" s="40">
+        <v>97.24</v>
+      </c>
+    </row>
+    <row r="49" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B49" s="25" t="s">
         <v>59</v>
       </c>
@@ -9890,8 +11950,29 @@
       <c r="W49" s="41">
         <v>3.42</v>
       </c>
-    </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y49" s="25">
+        <v>0.7</v>
+      </c>
+      <c r="Z49" s="32">
+        <v>97.98</v>
+      </c>
+      <c r="AA49" s="32">
+        <v>96.71</v>
+      </c>
+      <c r="AB49" s="32">
+        <v>97.18</v>
+      </c>
+      <c r="AC49" s="32">
+        <v>97.9</v>
+      </c>
+      <c r="AD49" s="32">
+        <v>97.61</v>
+      </c>
+      <c r="AE49" s="40">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B50" s="25" t="s">
         <v>62</v>
       </c>
@@ -9916,8 +11997,29 @@
       <c r="M50" s="1"/>
       <c r="P50" s="1"/>
       <c r="T50" s="1"/>
-    </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y50" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="Z50" s="20">
+        <v>98</v>
+      </c>
+      <c r="AA50" s="20">
+        <v>97.08</v>
+      </c>
+      <c r="AB50" s="20">
+        <v>97.45</v>
+      </c>
+      <c r="AC50" s="20">
+        <v>97.96</v>
+      </c>
+      <c r="AD50" s="20">
+        <v>97.75</v>
+      </c>
+      <c r="AE50" s="34">
+        <v>97.67</v>
+      </c>
+    </row>
+    <row r="51" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B51" s="25" t="s">
         <v>60</v>
       </c>
@@ -9957,8 +12059,29 @@
       <c r="P51" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y51" s="25">
+        <v>0.9</v>
+      </c>
+      <c r="Z51" s="20">
+        <v>98.02</v>
+      </c>
+      <c r="AA51" s="20">
+        <v>97.34</v>
+      </c>
+      <c r="AB51" s="20">
+        <v>97.63</v>
+      </c>
+      <c r="AC51" s="20">
+        <v>98</v>
+      </c>
+      <c r="AD51" s="20">
+        <v>97.84</v>
+      </c>
+      <c r="AE51" s="34">
+        <v>97.79</v>
+      </c>
+    </row>
+    <row r="52" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B52" s="25" t="s">
         <v>61</v>
       </c>
@@ -9998,8 +12121,29 @@
       <c r="P52" s="36" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y52" s="25">
+        <v>1</v>
+      </c>
+      <c r="Z52" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AA52" s="20">
+        <v>97.52</v>
+      </c>
+      <c r="AB52" s="20">
+        <v>97.75</v>
+      </c>
+      <c r="AC52" s="20">
+        <v>98.01</v>
+      </c>
+      <c r="AD52" s="20">
+        <v>97.9</v>
+      </c>
+      <c r="AE52" s="34">
+        <v>97.86</v>
+      </c>
+    </row>
+    <row r="53" spans="2:31" x14ac:dyDescent="0.25">
       <c r="J53" s="25">
         <v>1</v>
       </c>
@@ -10021,8 +12165,29 @@
       <c r="P53" s="34">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y53" s="25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z53" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AA53" s="20">
+        <v>97.65</v>
+      </c>
+      <c r="AB53" s="20">
+        <v>97.84</v>
+      </c>
+      <c r="AC53" s="20">
+        <v>98.02</v>
+      </c>
+      <c r="AD53" s="20">
+        <v>97.94</v>
+      </c>
+      <c r="AE53" s="34">
+        <v>97.92</v>
+      </c>
+    </row>
+    <row r="54" spans="2:31" x14ac:dyDescent="0.25">
       <c r="J54" s="25">
         <v>2</v>
       </c>
@@ -10044,8 +12209,29 @@
       <c r="P54" s="34">
         <v>1.19</v>
       </c>
-    </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y54" s="25">
+        <v>1.2</v>
+      </c>
+      <c r="Z54" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AA54" s="20">
+        <v>97.75</v>
+      </c>
+      <c r="AB54" s="20">
+        <v>97.9</v>
+      </c>
+      <c r="AC54" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AD54" s="20">
+        <v>97.97</v>
+      </c>
+      <c r="AE54" s="34">
+        <v>97.95</v>
+      </c>
+    </row>
+    <row r="55" spans="2:31" x14ac:dyDescent="0.25">
       <c r="J55" s="25">
         <v>3</v>
       </c>
@@ -10067,8 +12253,29 @@
       <c r="P55" s="34">
         <v>1.96</v>
       </c>
-    </row>
-    <row r="56" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y55" s="25">
+        <v>1.3</v>
+      </c>
+      <c r="Z55" s="20">
+        <v>98.04</v>
+      </c>
+      <c r="AA55" s="20">
+        <v>97.82</v>
+      </c>
+      <c r="AB55" s="20">
+        <v>97.94</v>
+      </c>
+      <c r="AC55" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AD55" s="20">
+        <v>97.99</v>
+      </c>
+      <c r="AE55" s="34">
+        <v>97.98</v>
+      </c>
+    </row>
+    <row r="56" spans="2:31" x14ac:dyDescent="0.25">
       <c r="J56" s="25">
         <v>4</v>
       </c>
@@ -10090,8 +12297,29 @@
       <c r="P56" s="34">
         <v>2.79</v>
       </c>
-    </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y56" s="25">
+        <v>1.4</v>
+      </c>
+      <c r="Z56" s="20">
+        <v>98.04</v>
+      </c>
+      <c r="AA56" s="20">
+        <v>97.87</v>
+      </c>
+      <c r="AB56" s="20">
+        <v>97.96</v>
+      </c>
+      <c r="AC56" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AD56" s="20">
+        <v>98</v>
+      </c>
+      <c r="AE56" s="34">
+        <v>97.99</v>
+      </c>
+    </row>
+    <row r="57" spans="2:31" x14ac:dyDescent="0.25">
       <c r="J57" s="25">
         <v>5</v>
       </c>
@@ -10113,8 +12341,29 @@
       <c r="P57" s="34">
         <v>3.65</v>
       </c>
-    </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y57" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="Z57" s="20">
+        <v>98.04</v>
+      </c>
+      <c r="AA57" s="20">
+        <v>97.91</v>
+      </c>
+      <c r="AB57" s="20">
+        <v>97.99</v>
+      </c>
+      <c r="AC57" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AD57" s="20">
+        <v>98.01</v>
+      </c>
+      <c r="AE57" s="34">
+        <v>98.01</v>
+      </c>
+    </row>
+    <row r="58" spans="2:31" x14ac:dyDescent="0.25">
       <c r="J58" s="25">
         <v>6</v>
       </c>
@@ -10136,8 +12385,29 @@
       <c r="P58" s="34">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y58" s="25">
+        <v>1.6</v>
+      </c>
+      <c r="Z58" s="20">
+        <v>98.04</v>
+      </c>
+      <c r="AA58" s="20">
+        <v>97.94</v>
+      </c>
+      <c r="AB58" s="20">
+        <v>98</v>
+      </c>
+      <c r="AC58" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AD58" s="20">
+        <v>98.02</v>
+      </c>
+      <c r="AE58" s="34">
+        <v>98.02</v>
+      </c>
+    </row>
+    <row r="59" spans="2:31" x14ac:dyDescent="0.25">
       <c r="J59" s="25">
         <v>7</v>
       </c>
@@ -10159,8 +12429,75 @@
       <c r="P59" s="35">
         <v>5.36</v>
       </c>
-    </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y59" s="25">
+        <v>1.7</v>
+      </c>
+      <c r="Z59" s="20">
+        <v>98.04</v>
+      </c>
+      <c r="AA59" s="20">
+        <v>97.97</v>
+      </c>
+      <c r="AB59" s="20">
+        <v>98.01</v>
+      </c>
+      <c r="AC59" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AD59" s="20">
+        <v>98.02</v>
+      </c>
+      <c r="AE59" s="34">
+        <v>98.02</v>
+      </c>
+    </row>
+    <row r="60" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="Y60" s="25">
+        <v>1.8</v>
+      </c>
+      <c r="Z60" s="20">
+        <v>98.04</v>
+      </c>
+      <c r="AA60" s="20">
+        <v>97.98</v>
+      </c>
+      <c r="AB60" s="20">
+        <v>98.02</v>
+      </c>
+      <c r="AC60" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AD60" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AE60" s="34">
+        <v>97.93</v>
+      </c>
+    </row>
+    <row r="61" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="Y61" s="25">
+        <v>1.9</v>
+      </c>
+      <c r="Z61" s="20">
+        <v>98.04</v>
+      </c>
+      <c r="AA61" s="20">
+        <v>98</v>
+      </c>
+      <c r="AB61" s="20">
+        <v>98.02</v>
+      </c>
+      <c r="AC61" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AD61" s="20">
+        <v>98.03</v>
+      </c>
+      <c r="AE61" s="34">
+        <v>97.93</v>
+      </c>
+    </row>
+    <row r="62" spans="2:31" x14ac:dyDescent="0.25">
       <c r="F62" t="s">
         <v>4</v>
       </c>
@@ -10171,8 +12508,29 @@
       <c r="I62" s="24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y62" s="25">
+        <v>2</v>
+      </c>
+      <c r="Z62" s="21">
+        <v>98.04</v>
+      </c>
+      <c r="AA62" s="21">
+        <v>98.01</v>
+      </c>
+      <c r="AB62" s="21">
+        <v>98.03</v>
+      </c>
+      <c r="AC62" s="21">
+        <v>98.03</v>
+      </c>
+      <c r="AD62" s="21">
+        <v>98.03</v>
+      </c>
+      <c r="AE62" s="34">
+        <v>97.93</v>
+      </c>
+    </row>
+    <row r="63" spans="2:31" x14ac:dyDescent="0.25">
       <c r="F63" t="s">
         <v>21</v>
       </c>
@@ -10185,8 +12543,11 @@
       <c r="I63" s="34">
         <v>14</v>
       </c>
-    </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="Y63" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="2:31" x14ac:dyDescent="0.25">
       <c r="G64" s="39">
         <v>1</v>
       </c>

</xml_diff>